<commit_message>
avances en tablero de control y modelado
</commit_message>
<xml_diff>
--- a/clasificacion a priori.xlsx
+++ b/clasificacion a priori.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Python\proyecto_grado_maestria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Python\proyecto_maestria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D430F35-9D02-4CA5-82F1-206D646D0BCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5422A66-99CC-4050-8613-D58C35E795F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="2220" windowWidth="26940" windowHeight="12050" xr2:uid="{D4E18D23-3CCB-4765-B467-5883BEADFEC5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D4E18D23-3CCB-4765-B467-5883BEADFEC5}"/>
   </bookViews>
   <sheets>
     <sheet name="detalle" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="84">
   <si>
     <t>v_Urban Blues Project pres. Michael Procter - Love Don't Live (Accapella).wav</t>
   </si>
@@ -275,13 +275,25 @@
   </si>
   <si>
     <t>v_Full Intention - America (I Love America) (Dub American Style).wav</t>
+  </si>
+  <si>
+    <t>Ebo Taylor &amp; Pat Thomas &amp; Henrik Schwarz -  Ene Nyame 'A' Mensuro (Henrik Schwarz Blend).wav</t>
+  </si>
+  <si>
+    <t>v_Future Force - What You Want (Rim Job Dub).wav</t>
+  </si>
+  <si>
+    <t>v_Urban Blues Project pres Michael Procter - Love Don't Live (U.B.P. Classic Mix).wav</t>
+  </si>
+  <si>
+    <t>pendiente clasificar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +305,12 @@
       <sz val="8"/>
       <color rgb="FF55595C"/>
       <name val="Nunito Sans"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -315,9 +333,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A54B060-479F-4280-AE8C-92F9E198E96F}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1302,7 +1323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
@@ -1313,7 +1334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>77</v>
       </c>
@@ -1324,7 +1345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>78</v>
       </c>
@@ -1335,7 +1356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>79</v>
       </c>
@@ -1346,40 +1367,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.4">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.4">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.4">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="G53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="G54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="G55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.4">

</xml_diff>